<commit_message>
header 기본 틀 / 예매페이지명 변경 (booking -> ticketing)
</commit_message>
<xml_diff>
--- a/키워드정리.xlsx
+++ b/키워드정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ParkBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9764699B-9DCE-4EFC-8896-729448CC2555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699820E7-D3FE-4FDB-A82D-EE42F5F5C387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3915" yWindow="1080" windowWidth="15435" windowHeight="13695" activeTab="1" xr2:uid="{942862D5-0A05-48F5-9FB3-9F83174FA707}"/>
   </bookViews>
@@ -380,11 +380,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>booking.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>timetableAdd.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ticketing.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DFF87-6D18-444E-9A0B-D8700475E296}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -984,7 +984,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1125,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I25" t="s">
         <v>15</v>

</xml_diff>